<commit_message>
Added script file and corrected student template
</commit_message>
<xml_diff>
--- a/templates/student_template.xlsx
+++ b/templates/student_template.xlsx
@@ -41,7 +41,7 @@
             <text:p>Name </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Roll No</text:p>
+            <text:p>Roll Number</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Email</text:p>
@@ -61,11 +61,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-02-22T18:51:45.649252052</meta:creation-date>
-    <dc:date>2025-02-22T18:53:14.009684638</dc:date>
-    <meta:editing-duration>PT1M28S</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
+    <dc:date>2025-02-23T13:40:22.036850108</dc:date>
+    <meta:editing-duration>PT1M42S</meta:editing-duration>
+    <meta:editing-cycles>2</meta:editing-cycles>
+    <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="4" meta:object-count="0"/>
-    <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
   </office:meta>
 </office:document-meta>
 </file>
@@ -83,8 +83,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -143,9 +143,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">lAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAtQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -157,6 +157,7 @@
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item-map-named config:name="ScriptConfiguration">
         <config:config-item-map-entry config:name="Sheet1">

</xml_diff>